<commit_message>
Adding White Noise measuremnets and a couple TNC measurements
</commit_message>
<xml_diff>
--- a/Laptop Output Levels.xlsx
+++ b/Laptop Output Levels.xlsx
@@ -24,12 +24,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Laptop Level</t>
   </si>
   <si>
-    <t>Vpp</t>
+    <t>Vpp Gen 200</t>
+  </si>
+  <si>
+    <t>VPP White</t>
+  </si>
+  <si>
+    <t>PK-232</t>
+  </si>
+  <si>
+    <t>PK-88</t>
+  </si>
+  <si>
+    <t>Kam</t>
   </si>
 </sst>
 </file>
@@ -133,7 +145,7 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -144,7 +156,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Vpp</c:v>
+                  <c:v>Vpp Gen 200</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -163,68 +175,71 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$22</c:f>
+              <c:f>Sheet1!$A$2:$A$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>35</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>45</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>55</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>65</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>70</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>75</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>80</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>85</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>90</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>95</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
@@ -232,74 +247,249 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$22</c:f>
+              <c:f>Sheet1!$B$2:$B$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
+                  <c:v>5.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>3.4000000000000002E-2</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>0.08</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.16200000000000001</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.246</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.35299999999999998</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.502</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.622</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.8</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>0.97599999999999998</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>1.1180000000000001</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>1.4059999999999999</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>1.585</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>1.7749999999999999</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>2.0049999999999999</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>2.2549999999999999</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>2.5</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>2.82</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>3.17</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>3.55</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>VPP White</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>6.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.3000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.3000000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.16700000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.251</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.372</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.65500000000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.73399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.1120000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.4379999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.41</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.635</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.0299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.2650000000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.56</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.88</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.2050000000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.68</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4.0999999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -309,11 +499,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="355997936"/>
-        <c:axId val="355999896"/>
+        <c:axId val="336467960"/>
+        <c:axId val="336466392"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="355997936"/>
+        <c:axId val="336467960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -370,12 +560,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="355999896"/>
+        <c:crossAx val="336466392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="355999896"/>
+        <c:axId val="336466392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -432,7 +622,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="355997936"/>
+        <c:crossAx val="336467960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -444,6 +634,38 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1041,20 +1263,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>328612</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>23812</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1335,10 +1557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection sqref="A1:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1346,180 +1568,255 @@
     <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2">
         <v>5.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5</v>
       </c>
       <c r="B3">
         <v>3.4000000000000002E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>3.3000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10</v>
       </c>
       <c r="B4">
         <v>0.08</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>8.3000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>15</v>
       </c>
       <c r="B5">
         <v>0.16200000000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>20</v>
       </c>
       <c r="B6">
         <v>0.246</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>0.251</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>25</v>
       </c>
       <c r="B7">
         <v>0.35299999999999998</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>0.372</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>30</v>
       </c>
       <c r="B8">
         <v>0.502</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>0.48</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>35</v>
       </c>
       <c r="B9">
         <v>0.622</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>0.65500000000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>40</v>
       </c>
       <c r="B10">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>0.73399999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>45</v>
       </c>
       <c r="B11">
         <v>0.97599999999999998</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>50</v>
       </c>
       <c r="B12">
         <v>1.1180000000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>1.1120000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>55</v>
       </c>
       <c r="B13">
         <v>1.4059999999999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>1.4379999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>60</v>
       </c>
       <c r="B14">
         <v>1.585</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>1.41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>65</v>
       </c>
       <c r="B15">
         <v>1.7749999999999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>1.635</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>70</v>
       </c>
       <c r="B16">
         <v>2.0049999999999999</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>2.0299999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>75</v>
       </c>
       <c r="B17">
         <v>2.2549999999999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>2.2650000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>80</v>
       </c>
       <c r="B18">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>85</v>
       </c>
       <c r="B19">
         <v>2.82</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>2.88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>90</v>
       </c>
       <c r="B20">
         <v>3.17</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>3.2050000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>95</v>
       </c>
       <c r="B21">
         <v>3.55</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>3.68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>100</v>
       </c>
       <c r="B22">
         <v>4</v>
+      </c>
+      <c r="C22">
+        <v>4.0999999999999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Saving some of the support documents
</commit_message>
<xml_diff>
--- a/Laptop Output Levels.xlsx
+++ b/Laptop Output Levels.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Laptop Level</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>Kam</t>
+  </si>
+  <si>
+    <t>MFJ-1278</t>
   </si>
 </sst>
 </file>
@@ -1560,7 +1563,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C22"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1636,6 +1639,9 @@
       <c r="C6">
         <v>0.251</v>
       </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">

</xml_diff>